<commit_message>
corrections made on homework section 2
</commit_message>
<xml_diff>
--- a/section2/ExcelHomework.xlsx
+++ b/section2/ExcelHomework.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyslo\Code\SavvyCoders\Homework\section2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0128E99F-695C-4980-9761-A224CF4EE4CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{07AFEEB3-AC73-469A-B326-76D2BA67C156}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Roster" sheetId="21" r:id="rId1"/>
@@ -29,7 +29,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="19" r:id="rId8"/>
+    <pivotCache cacheId="22" r:id="rId8"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2601" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2605" uniqueCount="196">
   <si>
     <t>Step</t>
   </si>
@@ -705,6 +705,12 @@
   <si>
     <t>Wal-Mart</t>
   </si>
+  <si>
+    <t>Jan</t>
+  </si>
+  <si>
+    <t>Feb</t>
+  </si>
 </sst>
 </file>
 
@@ -998,7 +1004,7 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1122,6 +1128,9 @@
     <xf numFmtId="0" fontId="15" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Comma" xfId="7" builtinId="3"/>
@@ -1134,7 +1143,162 @@
     <cellStyle name="Percent 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
     <cellStyle name="Style 1" xfId="6" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
   </cellStyles>
-  <dxfs count="35">
+  <dxfs count="57">
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <protection locked="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <family val="2"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <family val="2"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <family val="2"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <family val="2"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -3371,7 +3535,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Payments!$D$3</c:f>
+              <c:f>Payments!$C$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3392,9 +3556,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Payments!$A$4:$C$8</c:f>
+              <c:f>Payments!$A$4:$B$13</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="6"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>B1</c:v>
@@ -3404,6 +3568,23 @@
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>PC</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>B1</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>B2</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>PC</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Jan</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Feb</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -3416,18 +3597,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Payments!$D$4:$D$8</c:f>
+              <c:f>Payments!$C$4:$C$13</c:f>
               <c:numCache>
                 <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>64894.25</c:v>
+                  <c:v>30270.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>70</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>34624</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7993,8 +8183,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C747A03D-941B-49C8-99D0-ECF203354D40}" name="PivotTable2" cacheId="19" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2" fieldListSortAscending="1">
-  <location ref="A3:D8" firstHeaderRow="1" firstDataRow="1" firstDataCol="3"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C747A03D-941B-49C8-99D0-ECF203354D40}" name="PivotTable2" cacheId="22" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2" fieldListSortAscending="1">
+  <location ref="A3:C13" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
   <pivotFields count="11">
     <pivotField numFmtId="14" showAll="0"/>
     <pivotField showAll="0" sortType="descending">
@@ -8154,18 +8344,33 @@
   </pivotFields>
   <rowFields count="3">
     <field x="10"/>
+    <field x="8"/>
     <field x="6"/>
-    <field x="8"/>
   </rowFields>
-  <rowItems count="5">
+  <rowItems count="10">
     <i>
       <x v="2"/>
+      <x v="1"/>
+    </i>
+    <i r="2">
       <x/>
     </i>
-    <i r="1">
+    <i r="2">
       <x v="1"/>
     </i>
+    <i r="2">
+      <x v="2"/>
+    </i>
     <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i r="2">
       <x v="2"/>
     </i>
     <i t="default">
@@ -8182,46 +8387,46 @@
     <dataField name="Sum of Tax Inclusive Amount" fld="4" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="22">
-    <format dxfId="34">
+    <format dxfId="56">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="33">
+    <format dxfId="55">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="32">
+    <format dxfId="54">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="31">
+    <format dxfId="53">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="30">
+    <format dxfId="52">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="29">
+    <format dxfId="51">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="28">
+    <format dxfId="50">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="27">
+    <format dxfId="49">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="26">
+    <format dxfId="48">
       <pivotArea field="10" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="25">
-      <pivotArea field="8" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="2"/>
+    <format dxfId="47">
+      <pivotArea field="8" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="24">
+    <format dxfId="46">
       <pivotArea field="10" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="23">
-      <pivotArea field="8" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="2"/>
+    <format dxfId="45">
+      <pivotArea field="8" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="22">
+    <format dxfId="44">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="21">
+    <format dxfId="43">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="10" count="3">
@@ -8232,28 +8437,28 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="20">
+    <format dxfId="42">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="19">
-      <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
+    <format dxfId="41">
+      <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="2"/>
     </format>
-    <format dxfId="18">
-      <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
+    <format dxfId="40">
+      <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="2"/>
     </format>
-    <format dxfId="17">
-      <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
+    <format dxfId="39">
+      <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="2"/>
     </format>
-    <format dxfId="16">
+    <format dxfId="38">
       <pivotArea field="10" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="15">
-      <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
+    <format dxfId="37">
+      <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="2"/>
     </format>
-    <format dxfId="14">
-      <pivotArea field="8" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="2"/>
+    <format dxfId="36">
+      <pivotArea field="8" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="13">
+    <format dxfId="35">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
   </formats>
@@ -8281,18 +8486,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{20024602-86CA-4E00-B05D-3EC6222B50EE}" name="Table2" displayName="Table2" ref="A2:I210" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{20024602-86CA-4E00-B05D-3EC6222B50EE}" name="Table2" displayName="Table2" ref="A2:I210" totalsRowShown="0" headerRowDxfId="34" dataDxfId="32" headerRowBorderDxfId="33" tableBorderDxfId="31">
   <autoFilter ref="A2:I210" xr:uid="{20024602-86CA-4E00-B05D-3EC6222B50EE}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{49EF2A0F-1727-4655-B961-3129B370281A}" name="Document Date" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{554837F5-F7FD-4F0E-B670-4EEEEE8E5EC7}" name="Supplier" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{4B5F848B-537D-4B47-8736-9EAB23EFB964}" name="Reference" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{40E7F82E-2B52-46D0-803E-F6924CF35892}" name="Description" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{60AC2904-3B6D-402C-A387-F899EFB1ACC0}" name="Tax Inclusive Amount" dataDxfId="4" dataCellStyle="Comma"/>
-    <tableColumn id="6" xr3:uid="{7BE48675-D866-4989-AF6D-964A384F2DB3}" name="Tax Code" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{5DCBA414-9EF9-41E6-8407-C99896598773}" name="Bank Code" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{8FB084E8-3320-4977-84F5-7CE9616F2065}" name="Account Code" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{71DACAA5-A3E3-406C-923D-30DBC1AD7B50}" name="Payment Date" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{49EF2A0F-1727-4655-B961-3129B370281A}" name="Document Date" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{554837F5-F7FD-4F0E-B670-4EEEEE8E5EC7}" name="Supplier" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{4B5F848B-537D-4B47-8736-9EAB23EFB964}" name="Reference" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{40E7F82E-2B52-46D0-803E-F6924CF35892}" name="Description" dataDxfId="27"/>
+    <tableColumn id="5" xr3:uid="{60AC2904-3B6D-402C-A387-F899EFB1ACC0}" name="Tax Inclusive Amount" dataDxfId="26" dataCellStyle="Comma"/>
+    <tableColumn id="6" xr3:uid="{7BE48675-D866-4989-AF6D-964A384F2DB3}" name="Tax Code" dataDxfId="25"/>
+    <tableColumn id="7" xr3:uid="{5DCBA414-9EF9-41E6-8407-C99896598773}" name="Bank Code" dataDxfId="24"/>
+    <tableColumn id="8" xr3:uid="{8FB084E8-3320-4977-84F5-7CE9616F2065}" name="Account Code" dataDxfId="23"/>
+    <tableColumn id="9" xr3:uid="{71DACAA5-A3E3-406C-923D-30DBC1AD7B50}" name="Payment Date" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8591,8 +8796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A60BCBE4-FD6E-48F7-A916-77868B0707EA}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8849,8 +9054,8 @@
         <v>181</v>
       </c>
       <c r="B21" s="36">
-        <f>COUNT(B4:B14)</f>
-        <v>0</v>
+        <f>COUNTA(B4:B14)</f>
+        <v>11</v>
       </c>
       <c r="C21" s="36">
         <f>COUNT(C4:C14)</f>
@@ -8870,8 +9075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A3E3EDF-2482-4049-BA5D-2FB66799CC23}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9048,7 +9253,9 @@
   </sheetPr>
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -15283,17 +15490,17 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA2CD4B6-A3AC-473F-A4D7-22C614C017F7}">
-  <dimension ref="A2:D8"/>
+  <dimension ref="A2:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="14" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12.28515625" bestFit="1" customWidth="1"/>
@@ -15310,65 +15517,106 @@
     <col min="26" max="26" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" ht="38.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="38.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="44" t="s">
         <v>154</v>
       </c>
       <c r="B3" s="45" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="46" t="s">
+      <c r="C3" s="46" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="39" t="s">
         <v>157</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="35">
-        <v>64894.25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>194</v>
+      </c>
+      <c r="C4" s="35">
+        <v>30301.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="37"/>
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="35">
+        <v>30270.25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="37"/>
+      <c r="B6" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="35">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="38"/>
-      <c r="B6" s="29" t="s">
+      <c r="C6" s="35">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="37"/>
+      <c r="B7" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="29" t="s">
+      <c r="C7" s="35">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="37"/>
+      <c r="B8" s="29" t="s">
+        <v>195</v>
+      </c>
+      <c r="C8" s="35">
+        <v>34664</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="37"/>
+      <c r="B9" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="35">
+        <v>34624</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="37"/>
+      <c r="B10" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="35">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="38"/>
+      <c r="B11" s="50" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="29" t="s">
         <v>158</v>
       </c>
-      <c r="D7" s="35">
+      <c r="C12" s="35">
         <v>64965.25</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="34" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="34" t="s">
         <v>155</v>
       </c>
-      <c r="B8" s="36"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="35">
+      <c r="B13" s="36"/>
+      <c r="C13" s="35">
         <v>64965.25</v>
       </c>
     </row>

</xml_diff>